<commit_message>
a e b done
testes feitos
</commit_message>
<xml_diff>
--- a/Trabalho/estudoNN.xlsx
+++ b/Trabalho/estudoNN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25630"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\2 semestre\CR\aula4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E9291B4-9840-43B7-B4F8-6B8705BFCD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{314C3B79-3CC6-4F45-8E60-82400AFBD72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
   <si>
     <t>Número de camadas escondidas</t>
   </si>
@@ -67,127 +67,166 @@
     <t>tansig, purelin</t>
   </si>
   <si>
+    <t>trainlm</t>
+  </si>
+  <si>
+    <t>dividerand = {0.7, 0.15, 0.15}</t>
+  </si>
+  <si>
+    <t>66,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O número e dimensão das camadas encondidas influencia o desempenho? </t>
+  </si>
+  <si>
+    <t>Conf1</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>tansig, tansig, purelin</t>
+  </si>
+  <si>
+    <t>92,3</t>
+  </si>
+  <si>
+    <t>68,8</t>
+  </si>
+  <si>
+    <t>Conf2</t>
+  </si>
+  <si>
+    <t>25,25</t>
+  </si>
+  <si>
+    <t>64,4</t>
+  </si>
+  <si>
+    <t>Conf3</t>
+  </si>
+  <si>
+    <t>5,5,5,5,5,5</t>
+  </si>
+  <si>
+    <t>tansig, tansig, tansig, tansig, tansig, purelin</t>
+  </si>
+  <si>
+    <t>73,6</t>
+  </si>
+  <si>
+    <t>55,5</t>
+  </si>
+  <si>
+    <t>Conf4</t>
+  </si>
+  <si>
+    <t>10,10,10,10,10,10</t>
+  </si>
+  <si>
+    <t>90,6</t>
+  </si>
+  <si>
+    <t>25,25,25,25,25,25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A função de treino influencia o desempenho? </t>
+  </si>
+  <si>
+    <t>traingd</t>
+  </si>
+  <si>
+    <t>63,3</t>
+  </si>
+  <si>
+    <t>51,1</t>
+  </si>
+  <si>
+    <t>trainbfg</t>
+  </si>
+  <si>
+    <t>51,3</t>
+  </si>
+  <si>
+    <t>28,8</t>
+  </si>
+  <si>
     <t>traingdx</t>
   </si>
   <si>
-    <t>dividerand = {0.7, 0.15, 0.15}</t>
-  </si>
-  <si>
-    <t>87,1</t>
-  </si>
-  <si>
     <t>75,5</t>
   </si>
   <si>
-    <t xml:space="preserve">O número e dimensão das camadas encondidas influencia o desempenho? </t>
-  </si>
-  <si>
-    <t>Conf1</t>
-  </si>
-  <si>
-    <t>5, 5</t>
-  </si>
-  <si>
-    <t>tansig, tansig, purelin</t>
-  </si>
-  <si>
-    <t>83,3</t>
-  </si>
-  <si>
-    <t>82,2</t>
-  </si>
-  <si>
-    <t>Conf2</t>
-  </si>
-  <si>
-    <t>10,10</t>
-  </si>
-  <si>
-    <t>87,2</t>
-  </si>
-  <si>
-    <t>97,7</t>
-  </si>
-  <si>
-    <t>Conf3</t>
-  </si>
-  <si>
-    <t>5,5,5,5,5,5</t>
-  </si>
-  <si>
-    <t>tansig, tansig, tansig, tansig, tansig, purelin</t>
-  </si>
-  <si>
-    <t>84,4</t>
-  </si>
-  <si>
-    <t>Conf4</t>
-  </si>
-  <si>
-    <t>10,10,10,10,10,10</t>
-  </si>
-  <si>
-    <t>86,4</t>
-  </si>
-  <si>
-    <t>91,1</t>
-  </si>
-  <si>
-    <t>25,25,25,25,25,25</t>
-  </si>
-  <si>
-    <t>96,6</t>
+    <t>trainbr</t>
+  </si>
+  <si>
+    <t>Conf5</t>
+  </si>
+  <si>
+    <t>traincgf</t>
+  </si>
+  <si>
+    <t>78,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As funções de ativação influenciam o desempenho? </t>
+  </si>
+  <si>
+    <t>logsig, purelin</t>
+  </si>
+  <si>
+    <t>purelin, logsig</t>
+  </si>
+  <si>
+    <t>16,6</t>
+  </si>
+  <si>
+    <t>17,7</t>
+  </si>
+  <si>
+    <t>logsig, tansig</t>
+  </si>
+  <si>
+    <t>77,7</t>
+  </si>
+  <si>
+    <t>tansig, logsig</t>
+  </si>
+  <si>
+    <t>51,6</t>
+  </si>
+  <si>
+    <t>48,8</t>
+  </si>
+  <si>
+    <t>compet, elliotsig</t>
+  </si>
+  <si>
+    <t>11,1</t>
   </si>
   <si>
     <t>Conf6</t>
   </si>
   <si>
-    <t>50,50,50,50,50,50</t>
-  </si>
-  <si>
-    <t>96,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A função de treino influencia o desempenho? </t>
-  </si>
-  <si>
-    <t>traingd</t>
-  </si>
-  <si>
-    <t>93,7</t>
-  </si>
-  <si>
-    <t>95,5</t>
-  </si>
-  <si>
-    <t>trainbfg</t>
-  </si>
-  <si>
-    <t>86,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As funções de ativação influenciam o desempenho? </t>
-  </si>
-  <si>
-    <t>logsig, purelin</t>
-  </si>
-  <si>
-    <t>trainlm</t>
-  </si>
-  <si>
-    <t>95.65</t>
-  </si>
-  <si>
-    <t>tansig, logsig</t>
-  </si>
-  <si>
-    <t>66.6</t>
-  </si>
-  <si>
-    <t>69.56</t>
-  </si>
-  <si>
-    <t>Conf5</t>
+    <t>elliotsig, compet</t>
+  </si>
+  <si>
+    <t>Conf7</t>
+  </si>
+  <si>
+    <t>hardlim, satlin</t>
+  </si>
+  <si>
+    <t>18,3</t>
+  </si>
+  <si>
+    <t>15,5</t>
+  </si>
+  <si>
+    <t>Conf8</t>
+  </si>
+  <si>
+    <t>satlin, hardlim</t>
   </si>
   <si>
     <t xml:space="preserve">A divisão de exemplos pelos conjuntos influencia o desempenho? </t>
@@ -196,20 +235,38 @@
     <t>dividerand = {0.33, 0.33, 0.33}</t>
   </si>
   <si>
-    <t>33.3</t>
+    <t>75,3</t>
   </si>
   <si>
     <t>dividerand = {0.9, 0.05, 0.05}</t>
   </si>
   <si>
-    <t>62.5</t>
+    <t>dividerand = {0.5, 0.25, 0.25}</t>
+  </si>
+  <si>
+    <t>86,3</t>
+  </si>
+  <si>
+    <t>dividerand = {0.60, 0.20, 0.20}</t>
+  </si>
+  <si>
+    <t>dividerand = {0.40, 0.30, 0.30}</t>
+  </si>
+  <si>
+    <t>82,3</t>
+  </si>
+  <si>
+    <t>72,2</t>
+  </si>
+  <si>
+    <t>dividerand = {0.80, 0.10, 0.10}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +334,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -413,7 +477,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -445,6 +509,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -456,78 +526,78 @@
     </xf>
   </cellXfs>
   <cellStyles count="73">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -865,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -919,47 +989,47 @@
       <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4">
+        <v>90</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.95" customHeight="1"/>
     <row r="5" spans="1:9" ht="16.5" thickBot="1"/>
     <row r="6" spans="1:9" ht="56.1" customHeight="1" thickBot="1">
-      <c r="A6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
+      <c r="A6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>9</v>
@@ -969,51 +1039,51 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6">
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4">
+        <v>89</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="9">
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>9</v>
@@ -1023,24 +1093,24 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="9">
         <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>9</v>
@@ -1050,82 +1120,82 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="I10" s="5">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="9">
         <v>6</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4">
+        <v>90</v>
+      </c>
+      <c r="I11" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="56.1" customHeight="1">
+      <c r="A13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4" t="s">
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="I14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="9">
-        <v>6</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="56.1" customHeight="1">
-      <c r="A14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -1137,22 +1207,22 @@
         <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -1163,67 +1233,91 @@
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4">
+        <v>93</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4">
+        <v>96</v>
+      </c>
+      <c r="I17" s="5">
+        <v>73.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="5" t="s">
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="5">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="16.5" thickBot="1"/>
     <row r="21" spans="1:9" ht="56.1" customHeight="1" thickBot="1">
-      <c r="A21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="A21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -1232,235 +1326,392 @@
         <v>10</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="4">
-        <v>98</v>
-      </c>
-      <c r="I22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>10</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="5" t="s">
+    </row>
+    <row r="24" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="H24" s="4">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3">
+        <v>10</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="H25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <v>10</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="H26" s="4">
+        <v>25</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>10</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" ht="16.5" thickBot="1"/>
-    <row r="29" spans="1:9" ht="56.1" customHeight="1" thickBot="1">
-      <c r="A29" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-    </row>
-    <row r="30" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3">
-        <v>10</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="5">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>10</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="4">
-        <v>56</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="H27" s="4">
+        <v>18</v>
+      </c>
+      <c r="I27" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <v>10</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>10</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="4">
+        <v>18</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="56.1" customHeight="1">
+      <c r="A31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="5"/>
+      <c r="H32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="5">
+        <v>58</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="H33" s="4">
+        <v>96</v>
+      </c>
+      <c r="I33" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3">
+        <v>10</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="H34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="5"/>
+      <c r="H35" s="4">
+        <v>85</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3">
+        <v>10</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="39.950000000000003" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>10</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="4">
+        <v>94</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A13:I13"/>
     <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A31:I31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>